<commit_message>
Ajout audit Gemini et mise à jour de la configuration
</commit_message>
<xml_diff>
--- a/Excel et data/Copie de Acronymes_extraitsTL.xlsx
+++ b/Excel et data/Copie de Acronymes_extraitsTL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\932151754\Documents\Developpement POC Education nationnale\EDN1\Excel et data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46DB69B-0187-4B08-A019-8D2DF1B04C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D63F6F5-3915-4E35-B550-8EABA33E55CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ColonnesPôles!$A$1:$C$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Envoi initial'!$A$1:$B$280</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">ColonneAspectContextuel!$A$1:$C$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">ColonnesPôles!$A$1:$C$36</definedName>
   </definedNames>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="498">
   <si>
     <t>Acronyme</t>
   </si>
@@ -1089,15 +1090,6 @@
     <t>division des examens et concours</t>
   </si>
   <si>
-    <t>division des…</t>
-  </si>
-  <si>
-    <t>division des..</t>
-  </si>
-  <si>
-    <t>ce sont des services des rectorats</t>
-  </si>
-  <si>
     <t>direction générale des finances publiques</t>
   </si>
   <si>
@@ -1209,9 +1201,6 @@
     <t>numérique et sciences de l'ingénieur</t>
   </si>
   <si>
-    <t>professeur des écoles?</t>
-  </si>
-  <si>
     <t>Pôle Inclusif d’Accompagnement Localisé</t>
   </si>
   <si>
@@ -1284,9 +1273,6 @@
     <t>Conseil de discipline</t>
   </si>
   <si>
-    <t>Conditions générales de vente ?</t>
-  </si>
-  <si>
     <t>Corps interministériel à gestion ministérielle</t>
   </si>
   <si>
@@ -1338,9 +1324,6 @@
     <t>National (pôle de médiation)</t>
   </si>
   <si>
-    <t>Numérique ("problème lié au numérique)</t>
-  </si>
-  <si>
     <t>Outre mer</t>
   </si>
   <si>
@@ -1380,13 +1363,6 @@
     <t>Accompagnants éducatifs petite enfance</t>
   </si>
   <si>
-    <t>au sujet ?</t>
-  </si>
-  <si>
-    <t>Test de compétence en langue chinoise pour enfants (CCCC) ?
-Pas un sigle national. Comité de Coordination, de Concertation et de Communication?</t>
-  </si>
-  <si>
     <t>Conseil médical départemental</t>
   </si>
   <si>
@@ -1546,7 +1522,19 @@
     <t>CREPS</t>
   </si>
   <si>
-    <t>Centre régional d'enseignement physique et sportif !</t>
+    <t>Conditions générales de vente</t>
+  </si>
+  <si>
+    <t>Centre régional d'enseignement physique et sportif</t>
+  </si>
+  <si>
+    <t>division des… -&gt; ce sont des services des rectorats</t>
+  </si>
+  <si>
+    <t>Numérique ("problème lié au numérique")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">professeur des écoles ou initial du médiateur </t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1545,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1581,14 +1569,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1638,36 +1618,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1975,52 +1950,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F280"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D280"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="89.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="21" max="21" width="14.08984375" customWidth="1"/>
-    <col min="22" max="22" width="17.453125" customWidth="1"/>
+    <col min="19" max="19" width="14.08984375" customWidth="1"/>
+    <col min="20" max="20" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2028,7 +2001,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2036,7 +2009,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2044,7 +2017,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2052,7 +2025,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +2033,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2068,12 +2041,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2081,15 +2054,12 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2097,7 +2067,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2105,7 +2075,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2113,7 +2083,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2121,20 +2091,21 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2142,18 +2113,17 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2161,7 +2131,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2169,17 +2139,17 @@
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2187,7 +2157,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2195,15 +2165,15 @@
         <v>283</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2211,7 +2181,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2219,15 +2189,15 @@
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2235,7 +2205,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2243,7 +2213,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2251,7 +2221,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2259,7 +2229,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2267,7 +2237,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2275,7 +2245,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2283,16 +2253,13 @@
         <v>332</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="29" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="C41" s="13"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2300,15 +2267,15 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2316,7 +2283,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2324,20 +2291,20 @@
         <v>288</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2345,7 +2312,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2353,15 +2320,15 @@
         <v>289</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2369,15 +2336,15 @@
         <v>335</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2385,7 +2352,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2393,7 +2360,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2401,7 +2368,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2409,45 +2376,44 @@
         <v>338</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="3"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2455,7 +2421,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2463,7 +2429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2532,9 +2498,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>497</v>
-      </c>
-    </row>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>72</v>
@@ -2543,22 +2510,24 @@
         <v>340</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -2569,7 +2538,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -2577,15 +2546,15 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -2593,7 +2562,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -2601,15 +2570,15 @@
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B85" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>81</v>
       </c>
@@ -2617,7 +2586,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -2625,7 +2594,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -2633,12 +2602,12 @@
         <v>344</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -2646,15 +2615,15 @@
         <v>345</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -2662,15 +2631,15 @@
         <v>346</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>89</v>
       </c>
@@ -2678,107 +2647,100 @@
         <v>347</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>91</v>
       </c>
       <c r="B96" t="s">
         <v>348</v>
       </c>
-      <c r="C96" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="F96" s="11"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>349</v>
-      </c>
-      <c r="C97" s="11"/>
-      <c r="F97" s="11"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>349</v>
-      </c>
-      <c r="C98" s="11"/>
-      <c r="F98" s="11"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>349</v>
-      </c>
-      <c r="C99" s="11"/>
-      <c r="F99" s="11"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="D99" s="10"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>95</v>
       </c>
       <c r="B100" t="s">
-        <v>350</v>
-      </c>
-      <c r="C100" s="11"/>
-      <c r="F100" s="11"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="D100" s="10"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>96</v>
       </c>
       <c r="B101" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>98</v>
       </c>
       <c r="B103" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -2786,49 +2748,49 @@
         <v>295</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>103</v>
       </c>
       <c r="B108" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>105</v>
       </c>
       <c r="B110" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -2836,10 +2798,10 @@
         <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>109</v>
       </c>
@@ -2849,7 +2811,7 @@
         <v>110</v>
       </c>
       <c r="B115" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -2857,7 +2819,7 @@
         <v>111</v>
       </c>
       <c r="B116" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -2865,7 +2827,7 @@
         <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -2873,7 +2835,7 @@
         <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -2881,7 +2843,7 @@
         <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -2889,10 +2851,10 @@
         <v>115</v>
       </c>
       <c r="B120" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>116</v>
       </c>
@@ -2902,7 +2864,7 @@
         <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -2910,7 +2872,7 @@
         <v>118</v>
       </c>
       <c r="B123" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -2918,7 +2880,7 @@
         <v>119</v>
       </c>
       <c r="B124" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -2926,25 +2888,25 @@
         <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -2954,7 +2916,7 @@
         <v>125</v>
       </c>
       <c r="B130" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -2962,10 +2924,10 @@
         <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>127</v>
       </c>
@@ -2975,7 +2937,7 @@
         <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -2983,7 +2945,7 @@
         <v>129</v>
       </c>
       <c r="B134" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -2991,7 +2953,7 @@
         <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -3007,20 +2969,20 @@
         <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>135</v>
       </c>
@@ -3030,15 +2992,15 @@
         <v>136</v>
       </c>
       <c r="B141" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -3048,10 +3010,10 @@
         <v>139</v>
       </c>
       <c r="B144" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -3059,15 +3021,15 @@
         <v>297</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>141</v>
       </c>
       <c r="B146" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>142</v>
       </c>
@@ -3075,7 +3037,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>143</v>
       </c>
@@ -3083,63 +3045,63 @@
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>144</v>
       </c>
       <c r="B149" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>145</v>
       </c>
       <c r="B150" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>146</v>
       </c>
       <c r="B151" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>147</v>
       </c>
       <c r="B152" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>148</v>
       </c>
       <c r="B153" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>149</v>
       </c>
       <c r="B154" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>150</v>
       </c>
       <c r="B155" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>151</v>
       </c>
@@ -3147,36 +3109,34 @@
         <v>300</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>153</v>
       </c>
       <c r="B158" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C160" s="3"/>
-    </row>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>155</v>
       </c>
       <c r="B161" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -3184,7 +3144,7 @@
         <v>156</v>
       </c>
       <c r="B162" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -3192,15 +3152,16 @@
         <v>157</v>
       </c>
       <c r="B163" t="s">
-        <v>376</v>
-      </c>
-    </row>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>158</v>
       </c>
       <c r="B165" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
@@ -3208,7 +3169,7 @@
         <v>159</v>
       </c>
       <c r="B166" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -3216,7 +3177,7 @@
         <v>160</v>
       </c>
       <c r="B167" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -3224,7 +3185,7 @@
         <v>161</v>
       </c>
       <c r="B168" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -3232,15 +3193,15 @@
         <v>162</v>
       </c>
       <c r="B169" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>164</v>
       </c>
@@ -3250,7 +3211,7 @@
         <v>165</v>
       </c>
       <c r="B172" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -3258,7 +3219,7 @@
         <v>166</v>
       </c>
       <c r="B173" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -3266,7 +3227,7 @@
         <v>167</v>
       </c>
       <c r="B174" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -3290,15 +3251,15 @@
         <v>170</v>
       </c>
       <c r="B177" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>172</v>
       </c>
@@ -3308,10 +3269,10 @@
         <v>173</v>
       </c>
       <c r="B180" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>174</v>
       </c>
@@ -3321,7 +3282,7 @@
         <v>175</v>
       </c>
       <c r="B182" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -3337,7 +3298,7 @@
         <v>177</v>
       </c>
       <c r="B184" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -3353,7 +3314,7 @@
         <v>179</v>
       </c>
       <c r="B186" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -3369,15 +3330,15 @@
         <v>181</v>
       </c>
       <c r="B188" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>183</v>
       </c>
@@ -3395,7 +3356,7 @@
         <v>185</v>
       </c>
       <c r="B192" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
@@ -3411,7 +3372,7 @@
         <v>187</v>
       </c>
       <c r="B194" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -3419,7 +3380,7 @@
         <v>188</v>
       </c>
       <c r="B195" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
@@ -3435,7 +3396,7 @@
         <v>190</v>
       </c>
       <c r="B197" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
@@ -3446,12 +3407,12 @@
         <v>309</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>193</v>
       </c>
@@ -3469,7 +3430,7 @@
         <v>195</v>
       </c>
       <c r="B202" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
@@ -3477,15 +3438,16 @@
         <v>196</v>
       </c>
       <c r="B203" t="s">
-        <v>432</v>
-      </c>
-    </row>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>197</v>
       </c>
       <c r="B205" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
@@ -3496,7 +3458,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>199</v>
       </c>
@@ -3530,15 +3492,15 @@
         <v>203</v>
       </c>
       <c r="B211" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>205</v>
       </c>
@@ -3548,7 +3510,7 @@
         <v>206</v>
       </c>
       <c r="B214" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
@@ -3556,7 +3518,7 @@
         <v>207</v>
       </c>
       <c r="B215" t="s">
-        <v>389</v>
+        <v>497</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
@@ -3564,7 +3526,7 @@
         <v>208</v>
       </c>
       <c r="B216" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
@@ -3572,10 +3534,10 @@
         <v>209</v>
       </c>
       <c r="B217" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>210</v>
       </c>
@@ -3585,7 +3547,7 @@
         <v>211</v>
       </c>
       <c r="B219" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
@@ -3593,7 +3555,7 @@
         <v>212</v>
       </c>
       <c r="B220" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
@@ -3604,12 +3566,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>215</v>
       </c>
@@ -3619,7 +3581,7 @@
         <v>216</v>
       </c>
       <c r="B224" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
@@ -3627,7 +3589,7 @@
         <v>217</v>
       </c>
       <c r="B225" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
@@ -3635,7 +3597,7 @@
         <v>218</v>
       </c>
       <c r="B226" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
@@ -3643,7 +3605,7 @@
         <v>219</v>
       </c>
       <c r="B227" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
@@ -3651,7 +3613,7 @@
         <v>220</v>
       </c>
       <c r="B228" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
@@ -3659,7 +3621,7 @@
         <v>221</v>
       </c>
       <c r="B229" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
@@ -3667,7 +3629,7 @@
         <v>222</v>
       </c>
       <c r="B230" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
@@ -3683,7 +3645,7 @@
         <v>224</v>
       </c>
       <c r="B232" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
@@ -3699,7 +3661,7 @@
         <v>226</v>
       </c>
       <c r="B234" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
@@ -3715,7 +3677,7 @@
         <v>228</v>
       </c>
       <c r="B236" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
@@ -3723,23 +3685,24 @@
         <v>229</v>
       </c>
       <c r="B237" t="s">
-        <v>396</v>
-      </c>
-    </row>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>230</v>
       </c>
       <c r="B239" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>232</v>
       </c>
@@ -3749,15 +3712,15 @@
         <v>233</v>
       </c>
       <c r="B242" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>235</v>
       </c>
@@ -3767,7 +3730,7 @@
         <v>236</v>
       </c>
       <c r="B245" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
@@ -3775,7 +3738,7 @@
         <v>237</v>
       </c>
       <c r="B246" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -3783,7 +3746,7 @@
         <v>238</v>
       </c>
       <c r="B247" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
@@ -3791,7 +3754,7 @@
         <v>239</v>
       </c>
       <c r="B248" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -3799,7 +3762,7 @@
         <v>240</v>
       </c>
       <c r="B249" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
@@ -3807,7 +3770,7 @@
         <v>241</v>
       </c>
       <c r="B250" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -3815,7 +3778,7 @@
         <v>242</v>
       </c>
       <c r="B251" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
@@ -3823,7 +3786,7 @@
         <v>243</v>
       </c>
       <c r="B252" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
@@ -3831,7 +3794,7 @@
         <v>244</v>
       </c>
       <c r="B253" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
@@ -3839,7 +3802,7 @@
         <v>245</v>
       </c>
       <c r="B254" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
@@ -3847,10 +3810,10 @@
         <v>246</v>
       </c>
       <c r="B255" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>247</v>
       </c>
@@ -3868,7 +3831,7 @@
         <v>249</v>
       </c>
       <c r="B258" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
@@ -3876,7 +3839,7 @@
         <v>250</v>
       </c>
       <c r="B259" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
@@ -3884,7 +3847,7 @@
         <v>251</v>
       </c>
       <c r="B260" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
@@ -3892,7 +3855,7 @@
         <v>252</v>
       </c>
       <c r="B261" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
@@ -3903,17 +3866,17 @@
         <v>320</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>256</v>
       </c>
@@ -3923,7 +3886,7 @@
         <v>257</v>
       </c>
       <c r="B266" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
@@ -3939,15 +3902,15 @@
         <v>259</v>
       </c>
       <c r="B268" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>261</v>
       </c>
@@ -3957,7 +3920,7 @@
         <v>262</v>
       </c>
       <c r="B271" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
@@ -3968,7 +3931,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>264</v>
       </c>
@@ -3978,44 +3941,49 @@
         <v>265</v>
       </c>
       <c r="B274" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>271</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F96:F100"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="C96:C100"/>
+  <autoFilter ref="A1:B280" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="D96:D100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4035,347 +4003,347 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="5"/>
-    <col min="2" max="2" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.90625" style="5"/>
+    <col min="1" max="1" width="10.90625" style="3"/>
+    <col min="2" max="2" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C20" s="4" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="B33" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>474</v>
-      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="C34" s="6"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C36" xr:uid="{C35AB745-199A-46CC-9273-4D1E408B672E}"/>
@@ -4398,88 +4366,88 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="5"/>
-    <col min="2" max="2" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.90625" style="5"/>
+    <col min="1" max="1" width="10.90625" style="3"/>
+    <col min="2" max="2" width="11.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="C1" s="9" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="C5" s="14"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="C7" s="14"/>
+      <c r="B7" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>483</v>
+      <c r="B8" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>